<commit_message>
successed count multiple sheet in one time
</commit_message>
<xml_diff>
--- a/18egout.xlsx
+++ b/18egout.xlsx
@@ -1,13 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="1个月" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="2个月" sheetId="3" state="visible" r:id="rId3"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -728,6 +730,24 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
+  <dimension ref="A1:A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData/>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A1:AK18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1101,9 +1121,8 @@
         <v>0</v>
       </c>
       <c r="I4" t="n">
-        <v>4</v>
-      </c>
-      <c r="J4" t="s"/>
+        <v>0</v>
+      </c>
       <c r="K4" t="n">
         <v>0</v>
       </c>
@@ -1137,7 +1156,6 @@
       <c r="U4" t="n">
         <v>0</v>
       </c>
-      <c r="V4" t="s"/>
       <c r="W4" t="n">
         <v>0</v>
       </c>
@@ -1171,7 +1189,6 @@
       <c r="AG4" t="n">
         <v>0</v>
       </c>
-      <c r="AH4" t="s"/>
       <c r="AI4" t="n">
         <v>0</v>
       </c>
@@ -1179,7 +1196,7 @@
         <v>0</v>
       </c>
       <c r="AK4" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:37">
@@ -1321,7 +1338,7 @@
         <v>0</v>
       </c>
       <c r="I6" t="n">
-        <v>13</v>
+        <v>0</v>
       </c>
       <c r="J6" t="s">
         <v>68</v>
@@ -1395,7 +1412,6 @@
       <c r="AG6" t="s">
         <v>70</v>
       </c>
-      <c r="AH6" t="s"/>
       <c r="AI6" t="n">
         <v>0</v>
       </c>
@@ -1403,7 +1419,7 @@
         <v>0</v>
       </c>
       <c r="AK6" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:37">
@@ -1432,7 +1448,7 @@
         <v>4</v>
       </c>
       <c r="I7" t="n">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="J7" t="s">
         <v>75</v>
@@ -1470,7 +1486,6 @@
       <c r="U7" t="s">
         <v>70</v>
       </c>
-      <c r="V7" t="s"/>
       <c r="W7" t="n">
         <v>0</v>
       </c>
@@ -1504,7 +1519,6 @@
       <c r="AG7" t="n">
         <v>0</v>
       </c>
-      <c r="AH7" t="s"/>
       <c r="AI7" t="n">
         <v>0</v>
       </c>
@@ -1512,7 +1526,7 @@
         <v>0</v>
       </c>
       <c r="AK7" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:37">
@@ -1541,7 +1555,7 @@
         <v>2</v>
       </c>
       <c r="I8" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="J8" t="s">
         <v>80</v>
@@ -1615,7 +1629,6 @@
       <c r="AG8" t="s">
         <v>42</v>
       </c>
-      <c r="AH8" t="s"/>
       <c r="AI8" t="n">
         <v>0</v>
       </c>
@@ -1623,7 +1636,7 @@
         <v>0</v>
       </c>
       <c r="AK8" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:37">
@@ -1652,9 +1665,8 @@
         <v>0</v>
       </c>
       <c r="I9" t="n">
-        <v>3</v>
-      </c>
-      <c r="J9" t="s"/>
+        <v>0</v>
+      </c>
       <c r="K9" t="n">
         <v>0</v>
       </c>
@@ -1688,7 +1700,6 @@
       <c r="U9" t="n">
         <v>0</v>
       </c>
-      <c r="V9" t="s"/>
       <c r="W9" t="n">
         <v>0</v>
       </c>
@@ -1722,7 +1733,6 @@
       <c r="AG9" t="n">
         <v>0</v>
       </c>
-      <c r="AH9" t="s"/>
       <c r="AI9" t="n">
         <v>0</v>
       </c>
@@ -1730,7 +1740,7 @@
         <v>0</v>
       </c>
       <c r="AK9" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:37">
@@ -1749,7 +1759,6 @@
       <c r="E10" s="1" t="n">
         <v>43123</v>
       </c>
-      <c r="F10" t="s"/>
       <c r="G10" t="n">
         <v>0</v>
       </c>
@@ -1759,7 +1768,6 @@
       <c r="I10" t="n">
         <v>0</v>
       </c>
-      <c r="J10" t="s"/>
       <c r="K10" t="n">
         <v>0</v>
       </c>
@@ -1793,7 +1801,6 @@
       <c r="U10" t="n">
         <v>0</v>
       </c>
-      <c r="V10" t="s"/>
       <c r="W10" t="n">
         <v>0</v>
       </c>
@@ -1827,7 +1834,6 @@
       <c r="AG10" t="n">
         <v>0</v>
       </c>
-      <c r="AH10" t="s"/>
       <c r="AI10" t="n">
         <v>0</v>
       </c>
@@ -1835,7 +1841,7 @@
         <v>0</v>
       </c>
       <c r="AK10" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:37">
@@ -1864,9 +1870,8 @@
         <v>2</v>
       </c>
       <c r="I11" t="n">
-        <v>4</v>
-      </c>
-      <c r="J11" t="s"/>
+        <v>0</v>
+      </c>
       <c r="K11" t="n">
         <v>0</v>
       </c>
@@ -1900,7 +1905,6 @@
       <c r="U11" t="n">
         <v>0</v>
       </c>
-      <c r="V11" t="s"/>
       <c r="W11" t="n">
         <v>0</v>
       </c>
@@ -1934,7 +1938,6 @@
       <c r="AG11" t="n">
         <v>0</v>
       </c>
-      <c r="AH11" t="s"/>
       <c r="AI11" t="n">
         <v>0</v>
       </c>
@@ -1942,7 +1945,7 @@
         <v>0</v>
       </c>
       <c r="AK11" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:37">
@@ -1971,7 +1974,7 @@
         <v>0</v>
       </c>
       <c r="I12" t="n">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="J12" t="s">
         <v>97</v>
@@ -2045,7 +2048,6 @@
       <c r="AG12" t="s">
         <v>70</v>
       </c>
-      <c r="AH12" t="s"/>
       <c r="AI12" t="n">
         <v>0</v>
       </c>
@@ -2053,7 +2055,7 @@
         <v>0</v>
       </c>
       <c r="AK12" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:37">
@@ -2072,7 +2074,6 @@
       <c r="E13" s="1" t="n">
         <v>43126</v>
       </c>
-      <c r="F13" t="s"/>
       <c r="G13" t="n">
         <v>0</v>
       </c>
@@ -2082,7 +2083,6 @@
       <c r="I13" t="n">
         <v>0</v>
       </c>
-      <c r="J13" t="s"/>
       <c r="K13" t="n">
         <v>0</v>
       </c>
@@ -2116,7 +2116,6 @@
       <c r="U13" t="n">
         <v>0</v>
       </c>
-      <c r="V13" t="s"/>
       <c r="W13" t="n">
         <v>0</v>
       </c>
@@ -2150,7 +2149,6 @@
       <c r="AG13" t="n">
         <v>0</v>
       </c>
-      <c r="AH13" t="s"/>
       <c r="AI13" t="n">
         <v>0</v>
       </c>
@@ -2158,7 +2156,7 @@
         <v>0</v>
       </c>
       <c r="AK13" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="14" spans="1:37">
@@ -2177,7 +2175,6 @@
       <c r="E14" s="1" t="n">
         <v>43127</v>
       </c>
-      <c r="F14" t="s"/>
       <c r="G14" t="n">
         <v>0</v>
       </c>
@@ -2187,7 +2184,6 @@
       <c r="I14" t="n">
         <v>0</v>
       </c>
-      <c r="J14" t="s"/>
       <c r="K14" t="n">
         <v>0</v>
       </c>
@@ -2221,7 +2217,6 @@
       <c r="U14" t="n">
         <v>0</v>
       </c>
-      <c r="V14" t="s"/>
       <c r="W14" t="n">
         <v>0</v>
       </c>
@@ -2255,7 +2250,6 @@
       <c r="AG14" t="n">
         <v>0</v>
       </c>
-      <c r="AH14" t="s"/>
       <c r="AI14" t="n">
         <v>0</v>
       </c>
@@ -2263,7 +2257,7 @@
         <v>0</v>
       </c>
       <c r="AK14" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="15" spans="1:37">
@@ -2405,7 +2399,7 @@
         <v>0</v>
       </c>
       <c r="I16" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J16" t="s">
         <v>116</v>
@@ -2479,7 +2473,6 @@
       <c r="AG16" t="s">
         <v>70</v>
       </c>
-      <c r="AH16" t="s"/>
       <c r="AI16" t="n">
         <v>0</v>
       </c>
@@ -2487,7 +2480,7 @@
         <v>0</v>
       </c>
       <c r="AK16" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="17" spans="1:37">
@@ -2516,9 +2509,8 @@
         <v>0</v>
       </c>
       <c r="I17" t="n">
-        <v>1</v>
-      </c>
-      <c r="J17" t="s"/>
+        <v>0</v>
+      </c>
       <c r="K17" t="n">
         <v>0</v>
       </c>
@@ -2552,7 +2544,6 @@
       <c r="U17" t="n">
         <v>0</v>
       </c>
-      <c r="V17" t="s"/>
       <c r="W17" t="n">
         <v>0</v>
       </c>
@@ -2586,7 +2577,6 @@
       <c r="AG17" t="n">
         <v>0</v>
       </c>
-      <c r="AH17" t="s"/>
       <c r="AI17" t="n">
         <v>0</v>
       </c>
@@ -2594,7 +2584,7 @@
         <v>0</v>
       </c>
       <c r="AK17" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="18" spans="1:37">
@@ -2613,7 +2603,6 @@
       <c r="E18" s="1" t="n">
         <v>43131</v>
       </c>
-      <c r="F18" t="s"/>
       <c r="G18" t="n">
         <v>0</v>
       </c>
@@ -2623,7 +2612,6 @@
       <c r="I18" t="n">
         <v>0</v>
       </c>
-      <c r="J18" t="s"/>
       <c r="K18" t="n">
         <v>0</v>
       </c>
@@ -2657,7 +2645,6 @@
       <c r="U18" t="n">
         <v>0</v>
       </c>
-      <c r="V18" t="s"/>
       <c r="W18" t="n">
         <v>0</v>
       </c>
@@ -2691,7 +2678,6 @@
       <c r="AG18" t="n">
         <v>0</v>
       </c>
-      <c r="AH18" t="s"/>
       <c r="AI18" t="n">
         <v>0</v>
       </c>
@@ -2699,7 +2685,1735 @@
         <v>0</v>
       </c>
       <c r="AK18" t="n">
-        <v>0</v>
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:AK16"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:37">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" t="s">
+        <v>14</v>
+      </c>
+      <c r="P1" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>16</v>
+      </c>
+      <c r="R1" t="s">
+        <v>17</v>
+      </c>
+      <c r="S1" t="s">
+        <v>18</v>
+      </c>
+      <c r="T1" t="s">
+        <v>19</v>
+      </c>
+      <c r="U1" t="s">
+        <v>20</v>
+      </c>
+      <c r="V1" t="s">
+        <v>21</v>
+      </c>
+      <c r="W1" t="s">
+        <v>22</v>
+      </c>
+      <c r="X1" t="s">
+        <v>23</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>24</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>25</v>
+      </c>
+      <c r="AA1" t="s">
+        <v>26</v>
+      </c>
+      <c r="AB1" t="s">
+        <v>27</v>
+      </c>
+      <c r="AC1" t="s">
+        <v>28</v>
+      </c>
+      <c r="AD1" t="s">
+        <v>29</v>
+      </c>
+      <c r="AE1" t="s">
+        <v>30</v>
+      </c>
+      <c r="AF1" t="s">
+        <v>31</v>
+      </c>
+      <c r="AG1" t="s">
+        <v>32</v>
+      </c>
+      <c r="AH1" t="s">
+        <v>33</v>
+      </c>
+      <c r="AI1" t="s">
+        <v>34</v>
+      </c>
+      <c r="AJ1" t="s">
+        <v>35</v>
+      </c>
+      <c r="AK1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="2" spans="1:37">
+      <c r="A2" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>37</v>
+      </c>
+      <c r="C2" t="s">
+        <v>38</v>
+      </c>
+      <c r="D2" t="s">
+        <v>39</v>
+      </c>
+      <c r="E2" s="1" t="n">
+        <v>43114</v>
+      </c>
+      <c r="F2" t="s">
+        <v>40</v>
+      </c>
+      <c r="G2" t="n">
+        <v>15</v>
+      </c>
+      <c r="H2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I2" t="n">
+        <v>15</v>
+      </c>
+      <c r="J2" t="s">
+        <v>41</v>
+      </c>
+      <c r="K2" t="n">
+        <v>14</v>
+      </c>
+      <c r="L2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M2" t="n">
+        <v>14</v>
+      </c>
+      <c r="N2" t="n">
+        <v>11</v>
+      </c>
+      <c r="O2" t="n">
+        <v>1</v>
+      </c>
+      <c r="P2" t="n">
+        <v>2</v>
+      </c>
+      <c r="Q2" t="n">
+        <v>0</v>
+      </c>
+      <c r="R2" t="n">
+        <v>0</v>
+      </c>
+      <c r="S2" t="n">
+        <v>0</v>
+      </c>
+      <c r="T2" t="n">
+        <v>0</v>
+      </c>
+      <c r="U2" t="s">
+        <v>42</v>
+      </c>
+      <c r="V2" t="s">
+        <v>43</v>
+      </c>
+      <c r="W2" t="n">
+        <v>12</v>
+      </c>
+      <c r="X2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y2" t="n">
+        <v>12</v>
+      </c>
+      <c r="Z2" t="n">
+        <v>9</v>
+      </c>
+      <c r="AA2" t="n">
+        <v>1</v>
+      </c>
+      <c r="AB2" t="n">
+        <v>2</v>
+      </c>
+      <c r="AC2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AF2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG2" t="s">
+        <v>42</v>
+      </c>
+      <c r="AH2" t="s">
+        <v>44</v>
+      </c>
+      <c r="AI2" t="n">
+        <v>1</v>
+      </c>
+      <c r="AJ2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK2" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:37">
+      <c r="A3" t="n">
+        <v>4</v>
+      </c>
+      <c r="B3" t="s">
+        <v>53</v>
+      </c>
+      <c r="C3" t="s">
+        <v>54</v>
+      </c>
+      <c r="D3" t="s">
+        <v>55</v>
+      </c>
+      <c r="E3" s="1" t="n">
+        <v>43117</v>
+      </c>
+      <c r="F3" t="s">
+        <v>56</v>
+      </c>
+      <c r="G3" t="n">
+        <v>4</v>
+      </c>
+      <c r="H3" t="n">
+        <v>0</v>
+      </c>
+      <c r="I3" t="n">
+        <v>0</v>
+      </c>
+      <c r="K3" t="n">
+        <v>0</v>
+      </c>
+      <c r="L3" t="n">
+        <v>0</v>
+      </c>
+      <c r="M3" t="n">
+        <v>0</v>
+      </c>
+      <c r="N3" t="n">
+        <v>0</v>
+      </c>
+      <c r="O3" t="n">
+        <v>0</v>
+      </c>
+      <c r="P3" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q3" t="n">
+        <v>0</v>
+      </c>
+      <c r="R3" t="n">
+        <v>0</v>
+      </c>
+      <c r="S3" t="n">
+        <v>0</v>
+      </c>
+      <c r="T3" t="n">
+        <v>0</v>
+      </c>
+      <c r="U3" t="n">
+        <v>0</v>
+      </c>
+      <c r="W3" t="n">
+        <v>0</v>
+      </c>
+      <c r="X3" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y3" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AF3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AJ3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK3" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:37">
+      <c r="A4" t="n">
+        <v>5</v>
+      </c>
+      <c r="B4" t="s">
+        <v>57</v>
+      </c>
+      <c r="C4" t="s">
+        <v>58</v>
+      </c>
+      <c r="D4" t="s">
+        <v>59</v>
+      </c>
+      <c r="E4" s="1" t="n">
+        <v>43118</v>
+      </c>
+      <c r="F4" t="s">
+        <v>60</v>
+      </c>
+      <c r="G4" t="n">
+        <v>7</v>
+      </c>
+      <c r="H4" t="n">
+        <v>0</v>
+      </c>
+      <c r="I4" t="n">
+        <v>7</v>
+      </c>
+      <c r="J4" t="s">
+        <v>61</v>
+      </c>
+      <c r="K4" t="n">
+        <v>2</v>
+      </c>
+      <c r="L4" t="n">
+        <v>0</v>
+      </c>
+      <c r="M4" t="n">
+        <v>2</v>
+      </c>
+      <c r="N4" t="n">
+        <v>1</v>
+      </c>
+      <c r="O4" t="n">
+        <v>1</v>
+      </c>
+      <c r="P4" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q4" t="n">
+        <v>0</v>
+      </c>
+      <c r="R4" t="n">
+        <v>0</v>
+      </c>
+      <c r="S4" t="n">
+        <v>0</v>
+      </c>
+      <c r="T4" t="n">
+        <v>0</v>
+      </c>
+      <c r="U4" t="s">
+        <v>50</v>
+      </c>
+      <c r="V4" t="s">
+        <v>62</v>
+      </c>
+      <c r="W4" t="n">
+        <v>1</v>
+      </c>
+      <c r="X4" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y4" t="n">
+        <v>1</v>
+      </c>
+      <c r="Z4" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA4" t="n">
+        <v>1</v>
+      </c>
+      <c r="AB4" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC4" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD4" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE4" t="n">
+        <v>0</v>
+      </c>
+      <c r="AF4" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG4" t="s">
+        <v>50</v>
+      </c>
+      <c r="AH4" t="s">
+        <v>63</v>
+      </c>
+      <c r="AI4" t="n">
+        <v>1</v>
+      </c>
+      <c r="AJ4" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK4" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:37">
+      <c r="A5" t="n">
+        <v>6</v>
+      </c>
+      <c r="B5" t="s">
+        <v>64</v>
+      </c>
+      <c r="C5" t="s">
+        <v>65</v>
+      </c>
+      <c r="D5" t="s">
+        <v>66</v>
+      </c>
+      <c r="E5" s="1" t="n">
+        <v>43119</v>
+      </c>
+      <c r="F5" t="s">
+        <v>67</v>
+      </c>
+      <c r="G5" t="n">
+        <v>13</v>
+      </c>
+      <c r="H5" t="n">
+        <v>0</v>
+      </c>
+      <c r="I5" t="n">
+        <v>0</v>
+      </c>
+      <c r="J5" t="s">
+        <v>68</v>
+      </c>
+      <c r="K5" t="n">
+        <v>5</v>
+      </c>
+      <c r="L5" t="n">
+        <v>0</v>
+      </c>
+      <c r="M5" t="n">
+        <v>5</v>
+      </c>
+      <c r="N5" t="n">
+        <v>4</v>
+      </c>
+      <c r="O5" t="n">
+        <v>0</v>
+      </c>
+      <c r="P5" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q5" t="n">
+        <v>0</v>
+      </c>
+      <c r="R5" t="n">
+        <v>0</v>
+      </c>
+      <c r="S5" t="n">
+        <v>0</v>
+      </c>
+      <c r="T5" t="n">
+        <v>0</v>
+      </c>
+      <c r="U5" t="s">
+        <v>42</v>
+      </c>
+      <c r="V5" t="s">
+        <v>69</v>
+      </c>
+      <c r="W5" t="n">
+        <v>2</v>
+      </c>
+      <c r="X5" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y5" t="n">
+        <v>2</v>
+      </c>
+      <c r="Z5" t="n">
+        <v>2</v>
+      </c>
+      <c r="AA5" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB5" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC5" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD5" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE5" t="n">
+        <v>0</v>
+      </c>
+      <c r="AF5" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG5" t="s">
+        <v>70</v>
+      </c>
+      <c r="AI5" t="n">
+        <v>0</v>
+      </c>
+      <c r="AJ5" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK5" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:37">
+      <c r="A6" t="n">
+        <v>7</v>
+      </c>
+      <c r="B6" t="s">
+        <v>71</v>
+      </c>
+      <c r="C6" t="s">
+        <v>72</v>
+      </c>
+      <c r="D6" t="s">
+        <v>73</v>
+      </c>
+      <c r="E6" s="1" t="n">
+        <v>43120</v>
+      </c>
+      <c r="F6" t="s">
+        <v>74</v>
+      </c>
+      <c r="G6" t="n">
+        <v>12</v>
+      </c>
+      <c r="H6" t="n">
+        <v>4</v>
+      </c>
+      <c r="I6" t="n">
+        <v>0</v>
+      </c>
+      <c r="J6" t="s">
+        <v>75</v>
+      </c>
+      <c r="K6" t="n">
+        <v>1</v>
+      </c>
+      <c r="L6" t="n">
+        <v>0</v>
+      </c>
+      <c r="M6" t="n">
+        <v>1</v>
+      </c>
+      <c r="N6" t="n">
+        <v>1</v>
+      </c>
+      <c r="O6" t="n">
+        <v>0</v>
+      </c>
+      <c r="P6" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q6" t="n">
+        <v>0</v>
+      </c>
+      <c r="R6" t="n">
+        <v>0</v>
+      </c>
+      <c r="S6" t="n">
+        <v>0</v>
+      </c>
+      <c r="T6" t="n">
+        <v>0</v>
+      </c>
+      <c r="U6" t="s">
+        <v>70</v>
+      </c>
+      <c r="W6" t="n">
+        <v>0</v>
+      </c>
+      <c r="X6" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y6" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z6" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA6" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB6" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC6" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD6" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE6" t="n">
+        <v>0</v>
+      </c>
+      <c r="AF6" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG6" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI6" t="n">
+        <v>0</v>
+      </c>
+      <c r="AJ6" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK6" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:37">
+      <c r="A7" t="n">
+        <v>8</v>
+      </c>
+      <c r="B7" t="s">
+        <v>76</v>
+      </c>
+      <c r="C7" t="s">
+        <v>77</v>
+      </c>
+      <c r="D7" t="s">
+        <v>78</v>
+      </c>
+      <c r="E7" s="1" t="n">
+        <v>43121</v>
+      </c>
+      <c r="F7" t="s">
+        <v>79</v>
+      </c>
+      <c r="G7" t="n">
+        <v>5</v>
+      </c>
+      <c r="H7" t="n">
+        <v>2</v>
+      </c>
+      <c r="I7" t="n">
+        <v>0</v>
+      </c>
+      <c r="J7" t="s">
+        <v>80</v>
+      </c>
+      <c r="K7" t="n">
+        <v>2</v>
+      </c>
+      <c r="L7" t="n">
+        <v>0</v>
+      </c>
+      <c r="M7" t="n">
+        <v>2</v>
+      </c>
+      <c r="N7" t="n">
+        <v>1</v>
+      </c>
+      <c r="O7" t="n">
+        <v>0</v>
+      </c>
+      <c r="P7" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q7" t="n">
+        <v>0</v>
+      </c>
+      <c r="R7" t="n">
+        <v>0</v>
+      </c>
+      <c r="S7" t="n">
+        <v>0</v>
+      </c>
+      <c r="T7" t="n">
+        <v>0</v>
+      </c>
+      <c r="U7" t="s">
+        <v>42</v>
+      </c>
+      <c r="V7" t="s">
+        <v>81</v>
+      </c>
+      <c r="W7" t="n">
+        <v>2</v>
+      </c>
+      <c r="X7" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y7" t="n">
+        <v>2</v>
+      </c>
+      <c r="Z7" t="n">
+        <v>1</v>
+      </c>
+      <c r="AA7" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB7" t="n">
+        <v>1</v>
+      </c>
+      <c r="AC7" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD7" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE7" t="n">
+        <v>0</v>
+      </c>
+      <c r="AF7" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG7" t="s">
+        <v>42</v>
+      </c>
+      <c r="AI7" t="n">
+        <v>0</v>
+      </c>
+      <c r="AJ7" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK7" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:37">
+      <c r="A8" t="n">
+        <v>9</v>
+      </c>
+      <c r="B8" t="s">
+        <v>82</v>
+      </c>
+      <c r="C8" t="s">
+        <v>83</v>
+      </c>
+      <c r="D8" t="s">
+        <v>84</v>
+      </c>
+      <c r="E8" s="1" t="n">
+        <v>43122</v>
+      </c>
+      <c r="F8" t="s">
+        <v>85</v>
+      </c>
+      <c r="G8" t="n">
+        <v>3</v>
+      </c>
+      <c r="H8" t="n">
+        <v>0</v>
+      </c>
+      <c r="I8" t="n">
+        <v>0</v>
+      </c>
+      <c r="K8" t="n">
+        <v>0</v>
+      </c>
+      <c r="L8" t="n">
+        <v>0</v>
+      </c>
+      <c r="M8" t="n">
+        <v>0</v>
+      </c>
+      <c r="N8" t="n">
+        <v>0</v>
+      </c>
+      <c r="O8" t="n">
+        <v>0</v>
+      </c>
+      <c r="P8" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q8" t="n">
+        <v>0</v>
+      </c>
+      <c r="R8" t="n">
+        <v>0</v>
+      </c>
+      <c r="S8" t="n">
+        <v>0</v>
+      </c>
+      <c r="T8" t="n">
+        <v>0</v>
+      </c>
+      <c r="U8" t="n">
+        <v>0</v>
+      </c>
+      <c r="W8" t="n">
+        <v>0</v>
+      </c>
+      <c r="X8" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y8" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z8" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA8" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB8" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC8" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD8" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE8" t="n">
+        <v>0</v>
+      </c>
+      <c r="AF8" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG8" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI8" t="n">
+        <v>0</v>
+      </c>
+      <c r="AJ8" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK8" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:37">
+      <c r="A9" t="n">
+        <v>10</v>
+      </c>
+      <c r="B9" t="s">
+        <v>86</v>
+      </c>
+      <c r="C9" t="s">
+        <v>87</v>
+      </c>
+      <c r="D9" t="s">
+        <v>88</v>
+      </c>
+      <c r="E9" s="1" t="n">
+        <v>43123</v>
+      </c>
+      <c r="G9" t="n">
+        <v>0</v>
+      </c>
+      <c r="H9" t="n">
+        <v>0</v>
+      </c>
+      <c r="I9" t="n">
+        <v>0</v>
+      </c>
+      <c r="K9" t="n">
+        <v>0</v>
+      </c>
+      <c r="L9" t="n">
+        <v>0</v>
+      </c>
+      <c r="M9" t="n">
+        <v>0</v>
+      </c>
+      <c r="N9" t="n">
+        <v>0</v>
+      </c>
+      <c r="O9" t="n">
+        <v>0</v>
+      </c>
+      <c r="P9" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q9" t="n">
+        <v>0</v>
+      </c>
+      <c r="R9" t="n">
+        <v>0</v>
+      </c>
+      <c r="S9" t="n">
+        <v>0</v>
+      </c>
+      <c r="T9" t="n">
+        <v>0</v>
+      </c>
+      <c r="U9" t="n">
+        <v>0</v>
+      </c>
+      <c r="W9" t="n">
+        <v>0</v>
+      </c>
+      <c r="X9" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y9" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z9" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA9" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB9" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC9" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD9" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE9" t="n">
+        <v>0</v>
+      </c>
+      <c r="AF9" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG9" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI9" t="n">
+        <v>0</v>
+      </c>
+      <c r="AJ9" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK9" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:37">
+      <c r="A10" t="n">
+        <v>11</v>
+      </c>
+      <c r="B10" t="s">
+        <v>89</v>
+      </c>
+      <c r="C10" t="s">
+        <v>90</v>
+      </c>
+      <c r="D10" t="s">
+        <v>91</v>
+      </c>
+      <c r="E10" s="1" t="n">
+        <v>43124</v>
+      </c>
+      <c r="F10" t="s">
+        <v>92</v>
+      </c>
+      <c r="G10" t="n">
+        <v>6</v>
+      </c>
+      <c r="H10" t="n">
+        <v>2</v>
+      </c>
+      <c r="I10" t="n">
+        <v>0</v>
+      </c>
+      <c r="K10" t="n">
+        <v>0</v>
+      </c>
+      <c r="L10" t="n">
+        <v>0</v>
+      </c>
+      <c r="M10" t="n">
+        <v>0</v>
+      </c>
+      <c r="N10" t="n">
+        <v>0</v>
+      </c>
+      <c r="O10" t="n">
+        <v>0</v>
+      </c>
+      <c r="P10" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q10" t="n">
+        <v>0</v>
+      </c>
+      <c r="R10" t="n">
+        <v>0</v>
+      </c>
+      <c r="S10" t="n">
+        <v>0</v>
+      </c>
+      <c r="T10" t="n">
+        <v>0</v>
+      </c>
+      <c r="U10" t="n">
+        <v>0</v>
+      </c>
+      <c r="W10" t="n">
+        <v>0</v>
+      </c>
+      <c r="X10" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y10" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z10" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA10" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB10" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC10" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD10" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE10" t="n">
+        <v>0</v>
+      </c>
+      <c r="AF10" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG10" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI10" t="n">
+        <v>0</v>
+      </c>
+      <c r="AJ10" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK10" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:37">
+      <c r="A11" t="n">
+        <v>13</v>
+      </c>
+      <c r="B11" t="s">
+        <v>99</v>
+      </c>
+      <c r="C11" t="s">
+        <v>100</v>
+      </c>
+      <c r="D11" t="s">
+        <v>101</v>
+      </c>
+      <c r="E11" s="1" t="n">
+        <v>43126</v>
+      </c>
+      <c r="G11" t="n">
+        <v>0</v>
+      </c>
+      <c r="H11" t="n">
+        <v>0</v>
+      </c>
+      <c r="I11" t="n">
+        <v>0</v>
+      </c>
+      <c r="K11" t="n">
+        <v>0</v>
+      </c>
+      <c r="L11" t="n">
+        <v>0</v>
+      </c>
+      <c r="M11" t="n">
+        <v>0</v>
+      </c>
+      <c r="N11" t="n">
+        <v>0</v>
+      </c>
+      <c r="O11" t="n">
+        <v>0</v>
+      </c>
+      <c r="P11" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q11" t="n">
+        <v>0</v>
+      </c>
+      <c r="R11" t="n">
+        <v>0</v>
+      </c>
+      <c r="S11" t="n">
+        <v>0</v>
+      </c>
+      <c r="T11" t="n">
+        <v>0</v>
+      </c>
+      <c r="U11" t="n">
+        <v>0</v>
+      </c>
+      <c r="W11" t="n">
+        <v>0</v>
+      </c>
+      <c r="X11" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y11" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z11" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA11" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB11" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC11" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD11" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE11" t="n">
+        <v>0</v>
+      </c>
+      <c r="AF11" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG11" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI11" t="n">
+        <v>0</v>
+      </c>
+      <c r="AJ11" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK11" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:37">
+      <c r="A12" t="n">
+        <v>14</v>
+      </c>
+      <c r="B12" t="s">
+        <v>102</v>
+      </c>
+      <c r="C12" t="s">
+        <v>103</v>
+      </c>
+      <c r="D12" t="s">
+        <v>104</v>
+      </c>
+      <c r="E12" s="1" t="n">
+        <v>43127</v>
+      </c>
+      <c r="G12" t="n">
+        <v>0</v>
+      </c>
+      <c r="H12" t="n">
+        <v>0</v>
+      </c>
+      <c r="I12" t="n">
+        <v>0</v>
+      </c>
+      <c r="K12" t="n">
+        <v>0</v>
+      </c>
+      <c r="L12" t="n">
+        <v>0</v>
+      </c>
+      <c r="M12" t="n">
+        <v>0</v>
+      </c>
+      <c r="N12" t="n">
+        <v>0</v>
+      </c>
+      <c r="O12" t="n">
+        <v>0</v>
+      </c>
+      <c r="P12" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q12" t="n">
+        <v>0</v>
+      </c>
+      <c r="R12" t="n">
+        <v>0</v>
+      </c>
+      <c r="S12" t="n">
+        <v>0</v>
+      </c>
+      <c r="T12" t="n">
+        <v>0</v>
+      </c>
+      <c r="U12" t="n">
+        <v>0</v>
+      </c>
+      <c r="W12" t="n">
+        <v>0</v>
+      </c>
+      <c r="X12" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y12" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z12" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA12" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB12" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC12" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD12" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE12" t="n">
+        <v>0</v>
+      </c>
+      <c r="AF12" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG12" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI12" t="n">
+        <v>0</v>
+      </c>
+      <c r="AJ12" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK12" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:37">
+      <c r="A13" t="n">
+        <v>15</v>
+      </c>
+      <c r="B13" t="s">
+        <v>105</v>
+      </c>
+      <c r="C13" t="s">
+        <v>106</v>
+      </c>
+      <c r="D13" t="s">
+        <v>107</v>
+      </c>
+      <c r="E13" s="1" t="n">
+        <v>43128</v>
+      </c>
+      <c r="F13" t="s">
+        <v>108</v>
+      </c>
+      <c r="G13" t="n">
+        <v>19</v>
+      </c>
+      <c r="H13" t="n">
+        <v>0</v>
+      </c>
+      <c r="I13" t="n">
+        <v>19</v>
+      </c>
+      <c r="J13" t="s">
+        <v>109</v>
+      </c>
+      <c r="K13" t="n">
+        <v>4</v>
+      </c>
+      <c r="L13" t="n">
+        <v>0</v>
+      </c>
+      <c r="M13" t="n">
+        <v>4</v>
+      </c>
+      <c r="N13" t="n">
+        <v>3</v>
+      </c>
+      <c r="O13" t="n">
+        <v>1</v>
+      </c>
+      <c r="P13" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q13" t="n">
+        <v>0</v>
+      </c>
+      <c r="R13" t="n">
+        <v>0</v>
+      </c>
+      <c r="S13" t="n">
+        <v>0</v>
+      </c>
+      <c r="T13" t="n">
+        <v>0</v>
+      </c>
+      <c r="U13" t="s">
+        <v>50</v>
+      </c>
+      <c r="V13" t="s">
+        <v>110</v>
+      </c>
+      <c r="W13" t="n">
+        <v>2</v>
+      </c>
+      <c r="X13" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y13" t="n">
+        <v>2</v>
+      </c>
+      <c r="Z13" t="n">
+        <v>1</v>
+      </c>
+      <c r="AA13" t="n">
+        <v>1</v>
+      </c>
+      <c r="AB13" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC13" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD13" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE13" t="n">
+        <v>0</v>
+      </c>
+      <c r="AF13" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG13" t="s">
+        <v>50</v>
+      </c>
+      <c r="AH13" t="s">
+        <v>111</v>
+      </c>
+      <c r="AI13" t="n">
+        <v>1</v>
+      </c>
+      <c r="AJ13" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK13" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:37">
+      <c r="A14" t="n">
+        <v>16</v>
+      </c>
+      <c r="B14" t="s">
+        <v>112</v>
+      </c>
+      <c r="C14" t="s">
+        <v>113</v>
+      </c>
+      <c r="D14" t="s">
+        <v>114</v>
+      </c>
+      <c r="E14" s="1" t="n">
+        <v>43129</v>
+      </c>
+      <c r="F14" t="s">
+        <v>115</v>
+      </c>
+      <c r="G14" t="n">
+        <v>2</v>
+      </c>
+      <c r="H14" t="n">
+        <v>0</v>
+      </c>
+      <c r="I14" t="n">
+        <v>0</v>
+      </c>
+      <c r="J14" t="s">
+        <v>116</v>
+      </c>
+      <c r="K14" t="n">
+        <v>1</v>
+      </c>
+      <c r="L14" t="n">
+        <v>0</v>
+      </c>
+      <c r="M14" t="n">
+        <v>1</v>
+      </c>
+      <c r="N14" t="n">
+        <v>1</v>
+      </c>
+      <c r="O14" t="n">
+        <v>0</v>
+      </c>
+      <c r="P14" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q14" t="n">
+        <v>0</v>
+      </c>
+      <c r="R14" t="n">
+        <v>0</v>
+      </c>
+      <c r="S14" t="n">
+        <v>0</v>
+      </c>
+      <c r="T14" t="n">
+        <v>0</v>
+      </c>
+      <c r="U14" t="s">
+        <v>70</v>
+      </c>
+      <c r="V14" t="s">
+        <v>117</v>
+      </c>
+      <c r="W14" t="n">
+        <v>1</v>
+      </c>
+      <c r="X14" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y14" t="n">
+        <v>1</v>
+      </c>
+      <c r="Z14" t="n">
+        <v>1</v>
+      </c>
+      <c r="AA14" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB14" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC14" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD14" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE14" t="n">
+        <v>0</v>
+      </c>
+      <c r="AF14" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG14" t="s">
+        <v>70</v>
+      </c>
+      <c r="AI14" t="n">
+        <v>0</v>
+      </c>
+      <c r="AJ14" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK14" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:37">
+      <c r="A15" t="n">
+        <v>17</v>
+      </c>
+      <c r="B15" t="s">
+        <v>118</v>
+      </c>
+      <c r="C15" t="s">
+        <v>119</v>
+      </c>
+      <c r="D15" t="s">
+        <v>120</v>
+      </c>
+      <c r="E15" s="1" t="n">
+        <v>43130</v>
+      </c>
+      <c r="F15" t="s">
+        <v>121</v>
+      </c>
+      <c r="G15" t="n">
+        <v>1</v>
+      </c>
+      <c r="H15" t="n">
+        <v>0</v>
+      </c>
+      <c r="I15" t="n">
+        <v>0</v>
+      </c>
+      <c r="K15" t="n">
+        <v>0</v>
+      </c>
+      <c r="L15" t="n">
+        <v>0</v>
+      </c>
+      <c r="M15" t="n">
+        <v>0</v>
+      </c>
+      <c r="N15" t="n">
+        <v>0</v>
+      </c>
+      <c r="O15" t="n">
+        <v>0</v>
+      </c>
+      <c r="P15" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q15" t="n">
+        <v>0</v>
+      </c>
+      <c r="R15" t="n">
+        <v>0</v>
+      </c>
+      <c r="S15" t="n">
+        <v>0</v>
+      </c>
+      <c r="T15" t="n">
+        <v>0</v>
+      </c>
+      <c r="U15" t="n">
+        <v>0</v>
+      </c>
+      <c r="W15" t="n">
+        <v>0</v>
+      </c>
+      <c r="X15" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y15" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z15" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA15" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB15" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC15" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD15" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE15" t="n">
+        <v>0</v>
+      </c>
+      <c r="AF15" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG15" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI15" t="n">
+        <v>0</v>
+      </c>
+      <c r="AJ15" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK15" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:37">
+      <c r="A16" t="n">
+        <v>18</v>
+      </c>
+      <c r="B16" t="s">
+        <v>122</v>
+      </c>
+      <c r="C16" t="s">
+        <v>123</v>
+      </c>
+      <c r="D16" t="s">
+        <v>124</v>
+      </c>
+      <c r="E16" s="1" t="n">
+        <v>43131</v>
+      </c>
+      <c r="G16" t="n">
+        <v>0</v>
+      </c>
+      <c r="H16" t="n">
+        <v>0</v>
+      </c>
+      <c r="I16" t="n">
+        <v>0</v>
+      </c>
+      <c r="K16" t="n">
+        <v>0</v>
+      </c>
+      <c r="L16" t="n">
+        <v>0</v>
+      </c>
+      <c r="M16" t="n">
+        <v>0</v>
+      </c>
+      <c r="N16" t="n">
+        <v>0</v>
+      </c>
+      <c r="O16" t="n">
+        <v>0</v>
+      </c>
+      <c r="P16" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q16" t="n">
+        <v>0</v>
+      </c>
+      <c r="R16" t="n">
+        <v>0</v>
+      </c>
+      <c r="S16" t="n">
+        <v>0</v>
+      </c>
+      <c r="T16" t="n">
+        <v>0</v>
+      </c>
+      <c r="U16" t="n">
+        <v>0</v>
+      </c>
+      <c r="W16" t="n">
+        <v>0</v>
+      </c>
+      <c r="X16" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y16" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z16" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA16" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB16" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC16" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD16" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE16" t="n">
+        <v>0</v>
+      </c>
+      <c r="AF16" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG16" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI16" t="n">
+        <v>0</v>
+      </c>
+      <c r="AJ16" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK16" t="n">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>